<commit_message>
data cleanup in player_career_info_df completed for now
</commit_message>
<xml_diff>
--- a/smoy_winners.xlsx
+++ b/smoy_winners.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="205">
   <si>
     <t>season_ending_year_x</t>
   </si>
@@ -602,6 +602,9 @@
   </si>
   <si>
     <t>1982-83</t>
+  </si>
+  <si>
+    <t>Toni Kukoc</t>
   </si>
   <si>
     <t>C</t>
@@ -1197,7 +1200,7 @@
         <v>1999</v>
       </c>
       <c r="R2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="S2">
         <v>25</v>
@@ -1206,7 +1209,7 @@
         <v>5</v>
       </c>
       <c r="U2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V2" t="s">
         <v>129</v>
@@ -1290,10 +1293,10 @@
         <v>154</v>
       </c>
       <c r="AW2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY2">
         <v>2024</v>
@@ -1352,7 +1355,7 @@
         <v>1992</v>
       </c>
       <c r="R3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="S3">
         <v>31</v>
@@ -1361,7 +1364,7 @@
         <v>7</v>
       </c>
       <c r="U3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V3" t="s">
         <v>130</v>
@@ -1445,10 +1448,10 @@
         <v>155</v>
       </c>
       <c r="AW3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY3">
         <v>2023</v>
@@ -1507,7 +1510,7 @@
         <v>1999</v>
       </c>
       <c r="R4" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="S4">
         <v>23</v>
@@ -1516,7 +1519,7 @@
         <v>3</v>
       </c>
       <c r="U4" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V4" t="s">
         <v>131</v>
@@ -1600,10 +1603,10 @@
         <v>156</v>
       </c>
       <c r="AW4" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX4" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY4">
         <v>2022</v>
@@ -1662,7 +1665,7 @@
         <v>1992</v>
       </c>
       <c r="R5" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="S5">
         <v>29</v>
@@ -1671,7 +1674,7 @@
         <v>7</v>
       </c>
       <c r="U5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V5" t="s">
         <v>132</v>
@@ -1755,10 +1758,10 @@
         <v>157</v>
       </c>
       <c r="AW5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY5">
         <v>2021</v>
@@ -1817,7 +1820,7 @@
         <v>1993</v>
       </c>
       <c r="R6" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="S6">
         <v>27</v>
@@ -1826,7 +1829,7 @@
         <v>5</v>
       </c>
       <c r="U6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V6" t="s">
         <v>133</v>
@@ -1910,10 +1913,10 @@
         <v>158</v>
       </c>
       <c r="AW6" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX6" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY6">
         <v>2020</v>
@@ -1972,7 +1975,7 @@
         <v>1986</v>
       </c>
       <c r="R7" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="S7">
         <v>33</v>
@@ -1981,7 +1984,7 @@
         <v>14</v>
       </c>
       <c r="U7" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V7" t="s">
         <v>133</v>
@@ -2065,10 +2068,10 @@
         <v>159</v>
       </c>
       <c r="AW7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY7">
         <v>2019</v>
@@ -2127,7 +2130,7 @@
         <v>1986</v>
       </c>
       <c r="R8" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="S8">
         <v>32</v>
@@ -2136,7 +2139,7 @@
         <v>13</v>
       </c>
       <c r="U8" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V8" t="s">
         <v>133</v>
@@ -2220,10 +2223,10 @@
         <v>160</v>
       </c>
       <c r="AW8" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX8" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY8">
         <v>2018</v>
@@ -2282,7 +2285,7 @@
         <v>1988</v>
       </c>
       <c r="R9" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="S9">
         <v>29</v>
@@ -2291,7 +2294,7 @@
         <v>9</v>
       </c>
       <c r="U9" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V9" t="s">
         <v>134</v>
@@ -2375,10 +2378,10 @@
         <v>161</v>
       </c>
       <c r="AW9" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX9" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY9">
         <v>2017</v>
@@ -2437,7 +2440,7 @@
         <v>1980</v>
       </c>
       <c r="R10" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="S10">
         <v>36</v>
@@ -2446,7 +2449,7 @@
         <v>16</v>
       </c>
       <c r="U10" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V10" t="s">
         <v>133</v>
@@ -2530,10 +2533,10 @@
         <v>162</v>
       </c>
       <c r="AW10" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX10" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY10">
         <v>2016</v>
@@ -2592,7 +2595,7 @@
         <v>1986</v>
       </c>
       <c r="R11" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="S11">
         <v>29</v>
@@ -2601,7 +2604,7 @@
         <v>10</v>
       </c>
       <c r="U11" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V11" t="s">
         <v>135</v>
@@ -2685,10 +2688,10 @@
         <v>163</v>
       </c>
       <c r="AW11" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX11" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY11">
         <v>2015</v>
@@ -2747,7 +2750,7 @@
         <v>1980</v>
       </c>
       <c r="R12" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="S12">
         <v>34</v>
@@ -2756,7 +2759,7 @@
         <v>14</v>
       </c>
       <c r="U12" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V12" t="s">
         <v>133</v>
@@ -2840,10 +2843,10 @@
         <v>164</v>
       </c>
       <c r="AW12" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX12" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY12">
         <v>2014</v>
@@ -2902,7 +2905,7 @@
         <v>1985</v>
       </c>
       <c r="R13" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="S13">
         <v>28</v>
@@ -2911,7 +2914,7 @@
         <v>9</v>
       </c>
       <c r="U13" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V13" t="s">
         <v>136</v>
@@ -2995,10 +2998,10 @@
         <v>165</v>
       </c>
       <c r="AW13" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX13" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY13">
         <v>2013</v>
@@ -3057,7 +3060,7 @@
         <v>1989</v>
       </c>
       <c r="R14" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="S14">
         <v>23</v>
@@ -3066,7 +3069,7 @@
         <v>3</v>
       </c>
       <c r="U14" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V14" t="s">
         <v>137</v>
@@ -3150,10 +3153,10 @@
         <v>166</v>
       </c>
       <c r="AW14" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX14" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY14">
         <v>2012</v>
@@ -3212,7 +3215,7 @@
         <v>1979</v>
       </c>
       <c r="R15" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="S15">
         <v>32</v>
@@ -3221,7 +3224,7 @@
         <v>12</v>
       </c>
       <c r="U15" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V15" t="s">
         <v>138</v>
@@ -3305,10 +3308,10 @@
         <v>167</v>
       </c>
       <c r="AW15" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX15" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY15">
         <v>2011</v>
@@ -3367,7 +3370,7 @@
         <v>1980</v>
       </c>
       <c r="R16" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="S16">
         <v>30</v>
@@ -3376,7 +3379,7 @@
         <v>10</v>
       </c>
       <c r="U16" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V16" t="s">
         <v>139</v>
@@ -3460,10 +3463,10 @@
         <v>168</v>
       </c>
       <c r="AW16" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX16" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY16">
         <v>2010</v>
@@ -3522,7 +3525,7 @@
         <v>1977</v>
       </c>
       <c r="R17" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="S17">
         <v>32</v>
@@ -3531,7 +3534,7 @@
         <v>10</v>
       </c>
       <c r="U17" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V17" t="s">
         <v>140</v>
@@ -3615,10 +3618,10 @@
         <v>169</v>
       </c>
       <c r="AW17" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX17" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY17">
         <v>2009</v>
@@ -3677,7 +3680,7 @@
         <v>1977</v>
       </c>
       <c r="R18" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="S18">
         <v>31</v>
@@ -3686,7 +3689,7 @@
         <v>6</v>
       </c>
       <c r="U18" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V18" t="s">
         <v>141</v>
@@ -3770,10 +3773,10 @@
         <v>170</v>
       </c>
       <c r="AW18" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX18" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY18">
         <v>2008</v>
@@ -3832,7 +3835,7 @@
         <v>1982</v>
       </c>
       <c r="R19" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="S19">
         <v>25</v>
@@ -3841,7 +3844,7 @@
         <v>4</v>
       </c>
       <c r="U19" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V19" t="s">
         <v>142</v>
@@ -3925,10 +3928,10 @@
         <v>171</v>
       </c>
       <c r="AW19" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX19" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY19">
         <v>2007</v>
@@ -3987,7 +3990,7 @@
         <v>1980</v>
       </c>
       <c r="R20" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="S20">
         <v>26</v>
@@ -3996,7 +3999,7 @@
         <v>6</v>
       </c>
       <c r="U20" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V20" t="s">
         <v>143</v>
@@ -4080,10 +4083,10 @@
         <v>172</v>
       </c>
       <c r="AW20" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX20" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY20">
         <v>2006</v>
@@ -4142,7 +4145,7 @@
         <v>1983</v>
       </c>
       <c r="R21" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="S21">
         <v>22</v>
@@ -4151,7 +4154,7 @@
         <v>1</v>
       </c>
       <c r="U21" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V21" t="s">
         <v>144</v>
@@ -4235,10 +4238,10 @@
         <v>173</v>
       </c>
       <c r="AW21" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX21" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY21">
         <v>2005</v>
@@ -4297,7 +4300,7 @@
         <v>1976</v>
       </c>
       <c r="R22" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="S22">
         <v>28</v>
@@ -4306,7 +4309,7 @@
         <v>6</v>
       </c>
       <c r="U22" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V22" t="s">
         <v>140</v>
@@ -4390,10 +4393,10 @@
         <v>174</v>
       </c>
       <c r="AW22" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX22" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY22">
         <v>2004</v>
@@ -4452,7 +4455,7 @@
         <v>1973</v>
       </c>
       <c r="R23" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="S23">
         <v>30</v>
@@ -4461,7 +4464,7 @@
         <v>6</v>
       </c>
       <c r="U23" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V23" t="s">
         <v>145</v>
@@ -4545,10 +4548,10 @@
         <v>175</v>
       </c>
       <c r="AW23" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX23" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY23">
         <v>2003</v>
@@ -4607,7 +4610,7 @@
         <v>1973</v>
       </c>
       <c r="R24" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="S24">
         <v>29</v>
@@ -4616,7 +4619,7 @@
         <v>7</v>
       </c>
       <c r="U24" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V24" t="s">
         <v>146</v>
@@ -4700,10 +4703,10 @@
         <v>176</v>
       </c>
       <c r="AW24" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX24" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY24">
         <v>2002</v>
@@ -4762,7 +4765,7 @@
         <v>1972</v>
       </c>
       <c r="R25" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="S25">
         <v>29</v>
@@ -4771,7 +4774,7 @@
         <v>7</v>
       </c>
       <c r="U25" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V25" t="s">
         <v>147</v>
@@ -4855,10 +4858,10 @@
         <v>177</v>
       </c>
       <c r="AW25" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX25" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY25">
         <v>2001</v>
@@ -4917,7 +4920,7 @@
         <v>1971</v>
       </c>
       <c r="R26" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="S26">
         <v>29</v>
@@ -4926,7 +4929,7 @@
         <v>7</v>
       </c>
       <c r="U26" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V26" t="s">
         <v>142</v>
@@ -5010,10 +5013,10 @@
         <v>178</v>
       </c>
       <c r="AW26" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX26" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY26">
         <v>2000</v>
@@ -5072,7 +5075,7 @@
         <v>1968</v>
       </c>
       <c r="R27" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="S27">
         <v>31</v>
@@ -5081,7 +5084,7 @@
         <v>5</v>
       </c>
       <c r="U27" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V27" t="s">
         <v>148</v>
@@ -5165,10 +5168,10 @@
         <v>179</v>
       </c>
       <c r="AW27" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX27" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY27">
         <v>1999</v>
@@ -5227,7 +5230,7 @@
         <v>1966</v>
       </c>
       <c r="R28" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="S28">
         <v>32</v>
@@ -5236,7 +5239,7 @@
         <v>10</v>
       </c>
       <c r="U28" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V28" t="s">
         <v>142</v>
@@ -5320,10 +5323,10 @@
         <v>180</v>
       </c>
       <c r="AW28" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX28" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY28">
         <v>1998</v>
@@ -5382,7 +5385,7 @@
         <v>1965</v>
       </c>
       <c r="R29" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="S29">
         <v>32</v>
@@ -5391,7 +5394,7 @@
         <v>8</v>
       </c>
       <c r="U29" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V29" t="s">
         <v>136</v>
@@ -5475,10 +5478,10 @@
         <v>181</v>
       </c>
       <c r="AW29" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX29" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY29">
         <v>1997</v>
@@ -5531,13 +5534,13 @@
         <v>4901</v>
       </c>
       <c r="P30" t="s">
-        <v>118</v>
+        <v>196</v>
       </c>
       <c r="Q30">
         <v>1968</v>
       </c>
       <c r="R30" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="S30">
         <v>28</v>
@@ -5546,7 +5549,7 @@
         <v>3</v>
       </c>
       <c r="U30" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V30" t="s">
         <v>144</v>
@@ -5630,10 +5633,10 @@
         <v>182</v>
       </c>
       <c r="AW30" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX30" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY30">
         <v>1996</v>
@@ -5692,7 +5695,7 @@
         <v>1966</v>
       </c>
       <c r="R31" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="S31">
         <v>29</v>
@@ -5701,7 +5704,7 @@
         <v>6</v>
       </c>
       <c r="U31" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V31" t="s">
         <v>136</v>
@@ -5785,10 +5788,10 @@
         <v>183</v>
       </c>
       <c r="AW31" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX31" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY31">
         <v>1995</v>
@@ -5847,7 +5850,7 @@
         <v>1964</v>
       </c>
       <c r="R32" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="S32">
         <v>30</v>
@@ -5856,7 +5859,7 @@
         <v>8</v>
       </c>
       <c r="U32" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V32" t="s">
         <v>149</v>
@@ -5940,10 +5943,10 @@
         <v>184</v>
       </c>
       <c r="AW32" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX32" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY32">
         <v>1994</v>
@@ -6002,7 +6005,7 @@
         <v>1966</v>
       </c>
       <c r="R33" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="S33">
         <v>27</v>
@@ -6011,7 +6014,7 @@
         <v>4</v>
       </c>
       <c r="U33" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V33" t="s">
         <v>150</v>
@@ -6095,10 +6098,10 @@
         <v>185</v>
       </c>
       <c r="AW33" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX33" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY33">
         <v>1993</v>
@@ -6157,7 +6160,7 @@
         <v>1962</v>
       </c>
       <c r="R34" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="S34">
         <v>30</v>
@@ -6166,7 +6169,7 @@
         <v>7</v>
       </c>
       <c r="U34" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V34" t="s">
         <v>151</v>
@@ -6250,10 +6253,10 @@
         <v>186</v>
       </c>
       <c r="AW34" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX34" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY34">
         <v>1992</v>
@@ -6312,7 +6315,7 @@
         <v>1962</v>
       </c>
       <c r="R35" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="S35">
         <v>29</v>
@@ -6321,7 +6324,7 @@
         <v>6</v>
       </c>
       <c r="U35" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V35" t="s">
         <v>151</v>
@@ -6405,10 +6408,10 @@
         <v>187</v>
       </c>
       <c r="AW35" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX35" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY35">
         <v>1991</v>
@@ -6467,7 +6470,7 @@
         <v>1959</v>
       </c>
       <c r="R36" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="S36">
         <v>31</v>
@@ -6476,7 +6479,7 @@
         <v>8</v>
       </c>
       <c r="U36" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V36" t="s">
         <v>152</v>
@@ -6560,10 +6563,10 @@
         <v>188</v>
       </c>
       <c r="AW36" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX36" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY36">
         <v>1990</v>
@@ -6622,7 +6625,7 @@
         <v>1959</v>
       </c>
       <c r="R37" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="S37">
         <v>30</v>
@@ -6631,7 +6634,7 @@
         <v>8</v>
       </c>
       <c r="U37" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V37" t="s">
         <v>142</v>
@@ -6715,10 +6718,10 @@
         <v>189</v>
       </c>
       <c r="AW37" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX37" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY37">
         <v>1989</v>
@@ -6777,7 +6780,7 @@
         <v>1964</v>
       </c>
       <c r="R38" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="S38">
         <v>24</v>
@@ -6786,7 +6789,7 @@
         <v>2</v>
       </c>
       <c r="U38" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V38" t="s">
         <v>140</v>
@@ -6870,10 +6873,10 @@
         <v>190</v>
       </c>
       <c r="AW38" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="AX38" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY38">
         <v>1988</v>
@@ -6932,7 +6935,7 @@
         <v>1959</v>
       </c>
       <c r="R39" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="S39">
         <v>28</v>
@@ -6941,7 +6944,7 @@
         <v>5</v>
       </c>
       <c r="U39" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V39" t="s">
         <v>152</v>
@@ -7025,10 +7028,10 @@
         <v>191</v>
       </c>
       <c r="AW39" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX39" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY39">
         <v>1987</v>
@@ -7087,7 +7090,7 @@
         <v>1952</v>
       </c>
       <c r="R40" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="S40">
         <v>34</v>
@@ -7096,7 +7099,7 @@
         <v>9</v>
       </c>
       <c r="U40" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V40" t="s">
         <v>130</v>
@@ -7180,10 +7183,10 @@
         <v>192</v>
       </c>
       <c r="AW40" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX40" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY40">
         <v>1986</v>
@@ -7242,7 +7245,7 @@
         <v>1957</v>
       </c>
       <c r="R41" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="S41">
         <v>28</v>
@@ -7251,7 +7254,7 @@
         <v>5</v>
       </c>
       <c r="U41" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V41" t="s">
         <v>130</v>
@@ -7335,10 +7338,10 @@
         <v>193</v>
       </c>
       <c r="AW41" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX41" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY41">
         <v>1985</v>
@@ -7397,7 +7400,7 @@
         <v>1957</v>
       </c>
       <c r="R42" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="S42">
         <v>27</v>
@@ -7406,7 +7409,7 @@
         <v>4</v>
       </c>
       <c r="U42" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V42" t="s">
         <v>130</v>
@@ -7490,10 +7493,10 @@
         <v>194</v>
       </c>
       <c r="AW42" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX42" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY42">
         <v>1984</v>
@@ -7540,7 +7543,7 @@
         <v>1951</v>
       </c>
       <c r="R43" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="S43">
         <v>32</v>
@@ -7549,7 +7552,7 @@
         <v>9</v>
       </c>
       <c r="U43" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V43" t="s">
         <v>147</v>
@@ -7633,10 +7636,10 @@
         <v>195</v>
       </c>
       <c r="AW43" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AX43" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AY43">
         <v>1983</v>

</xml_diff>